<commit_message>
Now parsing boolean signals as well!
</commit_message>
<xml_diff>
--- a/StdCANSheet_Updated.xlsx
+++ b/StdCANSheet_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quickScripts\PythonPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD46A64-FECD-4CB4-A34A-663A7F6CDD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794B8E25-21E7-4333-93A4-B4D90AB2B444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdCANSheet_Updated" sheetId="1" r:id="rId1"/>
@@ -352,61 +352,61 @@
     <t>Pack3_IsolationActive_TF</t>
   </si>
   <si>
-    <t>Pack1_Fault_BatteryCAN</t>
-  </si>
-  <si>
     <t>boolean</t>
   </si>
   <si>
-    <t>Pack1_Fault_Contactor</t>
-  </si>
-  <si>
-    <t>Pack1_Fault_CurrentSensor</t>
-  </si>
-  <si>
-    <t>Pack1_Fault_DCLinkOverVoltage</t>
-  </si>
-  <si>
-    <t>Pack1_Fault_OvercurrentCharge</t>
-  </si>
-  <si>
-    <t>Pack1_Fault_OvercurrentDischarge</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_BatteryCAN</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_Contactor</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_CurrentSensor</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_DCLinkOverVoltage</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_OvercurrentCharge</t>
-  </si>
-  <si>
-    <t>Pack2_Fault_OvercurrentDischarge</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_BatteryCAN</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_Contactor</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_CurrentSensor</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_DCLinkOverVoltage</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_OvercurrentCharge</t>
-  </si>
-  <si>
-    <t>Pack3_Fault_OvercurrentDischarge</t>
+    <t>Pack1_Fault_BatteryCAN_TF</t>
+  </si>
+  <si>
+    <t>Pack1_Fault_Contactor_TF</t>
+  </si>
+  <si>
+    <t>Pack1_Fault_CurrentSensor_TF</t>
+  </si>
+  <si>
+    <t>Pack1_Fault_DCLinkOverVoltage_TF</t>
+  </si>
+  <si>
+    <t>Pack1_Fault_OvercurrentCharge_TF</t>
+  </si>
+  <si>
+    <t>Pack1_Fault_OvercurrentDischarge_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_BatteryCAN_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_Contactor_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_CurrentSensor_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_DCLinkOverVoltage_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_OvercurrentCharge_TF</t>
+  </si>
+  <si>
+    <t>Pack2_Fault_OvercurrentDischarge_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_BatteryCAN_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_Contactor_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_CurrentSensor_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_DCLinkOverVoltage_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_OvercurrentCharge_TF</t>
+  </si>
+  <si>
+    <t>Pack3_Fault_OvercurrentDischarge_TF</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,8 @@
   <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2913,19 +2914,19 @@
         <v>3</v>
       </c>
       <c r="B75" t="s">
+        <v>111</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
         <v>110</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-      <c r="H75">
-        <v>1</v>
-      </c>
-      <c r="I75" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2945,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -2965,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -2985,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -3005,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="I79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -3025,7 +3026,7 @@
         <v>1</v>
       </c>
       <c r="I80" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3033,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F81">
         <v>6</v>
@@ -3045,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="I81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -3082,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
@@ -3102,7 +3103,7 @@
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
@@ -3122,7 +3123,7 @@
         <v>1</v>
       </c>
       <c r="I85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -3142,7 +3143,7 @@
         <v>1</v>
       </c>
       <c r="I86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -3162,7 +3163,7 @@
         <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -3182,7 +3183,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
@@ -3202,7 +3203,7 @@
         <v>1</v>
       </c>
       <c r="I89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -3239,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="I91" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
@@ -3259,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -3279,7 +3280,7 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
@@ -3299,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
@@ -3319,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
@@ -3339,7 +3340,7 @@
         <v>1</v>
       </c>
       <c r="I96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
@@ -3359,7 +3360,7 @@
         <v>1</v>
       </c>
       <c r="I97" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Now working off of .xlsx sheet instead of .csv!
</commit_message>
<xml_diff>
--- a/StdCANSheet_Updated.xlsx
+++ b/StdCANSheet_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quickScripts\PythonPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794B8E25-21E7-4333-93A4-B4D90AB2B444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252778D2-1517-4BF1-8DDA-2E3A4E3E6E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdCANSheet_Updated" sheetId="1" r:id="rId1"/>
@@ -899,10 +899,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1268,17 +1270,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1324,7 +1327,7 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>128</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1341,13 +1344,13 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
         <v>16</v>
       </c>
       <c r="I3">
@@ -1367,13 +1370,13 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
         <v>16</v>
       </c>
       <c r="I4">
@@ -1393,13 +1396,13 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
         <v>16</v>
       </c>
       <c r="I5">
@@ -1419,7 +1422,7 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>128</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1428,6 +1431,9 @@
       <c r="E6" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1436,13 +1442,13 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
         <v>16</v>
       </c>
       <c r="I7">
@@ -1462,13 +1468,13 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
         <v>16</v>
       </c>
       <c r="I8">
@@ -1488,13 +1494,13 @@
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>5</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
         <v>16</v>
       </c>
       <c r="I9">
@@ -1514,7 +1520,7 @@
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>128</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1523,6 +1529,9 @@
       <c r="E10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1531,13 +1540,13 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
         <v>16</v>
       </c>
       <c r="I11">
@@ -1557,13 +1566,13 @@
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
         <v>16</v>
       </c>
       <c r="I12">
@@ -1583,13 +1592,13 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <v>5</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
         <v>16</v>
       </c>
       <c r="I13">
@@ -1609,7 +1618,7 @@
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>160</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1618,6 +1627,9 @@
       <c r="E14" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1626,13 +1638,13 @@
       <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
         <v>4</v>
       </c>
       <c r="I15" t="s">
@@ -1646,13 +1658,13 @@
       <c r="B16" t="s">
         <v>71</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="4">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4">
         <v>5</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>4</v>
       </c>
       <c r="I16" t="s">
@@ -1666,7 +1678,7 @@
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>161</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1675,6 +1687,9 @@
       <c r="E17" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1683,13 +1698,13 @@
       <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4">
         <v>4</v>
       </c>
       <c r="I18" t="s">
@@ -1703,13 +1718,13 @@
       <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4">
         <v>5</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>4</v>
       </c>
       <c r="I19" t="s">
@@ -1723,7 +1738,7 @@
       <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>162</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1732,6 +1747,9 @@
       <c r="E20" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1740,13 +1758,13 @@
       <c r="B21" t="s">
         <v>74</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
         <v>4</v>
       </c>
       <c r="I21" t="s">
@@ -1760,13 +1778,13 @@
       <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
         <v>5</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="4">
         <v>4</v>
       </c>
       <c r="I22" t="s">
@@ -1780,7 +1798,7 @@
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>896</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1789,6 +1807,9 @@
       <c r="E23" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1797,13 +1818,13 @@
       <c r="B24" t="s">
         <v>79</v>
       </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>3</v>
-      </c>
-      <c r="H24">
+      <c r="F24" s="4">
+        <v>2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3</v>
+      </c>
+      <c r="H24" s="4">
         <v>9</v>
       </c>
       <c r="I24" s="2">
@@ -1820,7 +1841,7 @@
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <v>897</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1829,6 +1850,9 @@
       <c r="E25" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1837,13 +1861,13 @@
       <c r="B26" t="s">
         <v>81</v>
       </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
-      <c r="H26">
+      <c r="F26" s="4">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4">
         <v>9</v>
       </c>
       <c r="I26" s="2">
@@ -1860,7 +1884,7 @@
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="3">
         <v>898</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1869,6 +1893,9 @@
       <c r="E27" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1877,13 +1904,13 @@
       <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-      <c r="H28">
+      <c r="F28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+      <c r="H28" s="4">
         <v>9</v>
       </c>
       <c r="I28" s="2">
@@ -1900,7 +1927,7 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="3">
         <v>352</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1909,6 +1936,9 @@
       <c r="E29" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1917,13 +1947,13 @@
       <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4">
         <v>16</v>
       </c>
       <c r="I30">
@@ -1943,13 +1973,13 @@
       <c r="B31" t="s">
         <v>84</v>
       </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
+      <c r="F31" s="4">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1</v>
+      </c>
+      <c r="H31" s="4">
         <v>16</v>
       </c>
       <c r="I31">
@@ -1969,7 +1999,7 @@
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="3">
         <v>353</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1978,6 +2008,9 @@
       <c r="E32" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -1986,13 +2019,13 @@
       <c r="B33" t="s">
         <v>85</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4">
         <v>16</v>
       </c>
       <c r="I33">
@@ -2012,13 +2045,13 @@
       <c r="B34" t="s">
         <v>86</v>
       </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
+      <c r="F34" s="4">
+        <v>3</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4">
         <v>16</v>
       </c>
       <c r="I34">
@@ -2038,7 +2071,7 @@
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>354</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -2047,6 +2080,9 @@
       <c r="E35" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -2055,13 +2091,13 @@
       <c r="B36" t="s">
         <v>87</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4">
         <v>16</v>
       </c>
       <c r="I36">
@@ -2081,13 +2117,13 @@
       <c r="B37" t="s">
         <v>88</v>
       </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
+      <c r="F37" s="4">
+        <v>3</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1</v>
+      </c>
+      <c r="H37" s="4">
         <v>16</v>
       </c>
       <c r="I37">
@@ -2107,7 +2143,7 @@
       <c r="B38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>288</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -2116,6 +2152,9 @@
       <c r="E38" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -2124,13 +2163,13 @@
       <c r="B39" t="s">
         <v>55</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1</v>
+      </c>
+      <c r="H39" s="4">
         <v>16</v>
       </c>
       <c r="I39">
@@ -2150,13 +2189,13 @@
       <c r="B40" t="s">
         <v>56</v>
       </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
+      <c r="F40" s="4">
+        <v>3</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1</v>
+      </c>
+      <c r="H40" s="4">
         <v>16</v>
       </c>
       <c r="I40">
@@ -2176,7 +2215,7 @@
       <c r="B41" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="3">
         <v>289</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2185,6 +2224,9 @@
       <c r="E41" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -2193,13 +2235,13 @@
       <c r="B42" t="s">
         <v>62</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>1</v>
-      </c>
-      <c r="H42">
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1</v>
+      </c>
+      <c r="H42" s="4">
         <v>16</v>
       </c>
       <c r="I42">
@@ -2219,13 +2261,13 @@
       <c r="B43" t="s">
         <v>63</v>
       </c>
-      <c r="F43">
-        <v>3</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
+      <c r="F43" s="4">
+        <v>3</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4">
         <v>16</v>
       </c>
       <c r="I43">
@@ -2245,7 +2287,7 @@
       <c r="B44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="3">
         <v>290</v>
       </c>
       <c r="D44" s="1" t="s">
@@ -2254,6 +2296,9 @@
       <c r="E44" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
@@ -2262,13 +2307,13 @@
       <c r="B45" t="s">
         <v>64</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1</v>
+      </c>
+      <c r="H45" s="4">
         <v>16</v>
       </c>
       <c r="I45">
@@ -2288,13 +2333,13 @@
       <c r="B46" t="s">
         <v>65</v>
       </c>
-      <c r="F46">
-        <v>3</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
+      <c r="F46" s="4">
+        <v>3</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1</v>
+      </c>
+      <c r="H46" s="4">
         <v>16</v>
       </c>
       <c r="I46">
@@ -2314,7 +2359,7 @@
       <c r="B47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="3">
         <v>608</v>
       </c>
       <c r="D47" s="1" t="s">
@@ -2323,6 +2368,9 @@
       <c r="E47" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -2331,13 +2379,13 @@
       <c r="B48" t="s">
         <v>89</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48">
+      <c r="F48" s="4">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4">
         <v>16</v>
       </c>
       <c r="I48">
@@ -2357,13 +2405,13 @@
       <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
+      <c r="F49" s="4">
+        <v>3</v>
+      </c>
+      <c r="G49" s="4">
+        <v>1</v>
+      </c>
+      <c r="H49" s="4">
         <v>16</v>
       </c>
       <c r="I49">
@@ -2383,13 +2431,13 @@
       <c r="B50" t="s">
         <v>91</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="4">
         <v>5</v>
       </c>
-      <c r="G50">
-        <v>1</v>
-      </c>
-      <c r="H50">
+      <c r="G50" s="4">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4">
         <v>16</v>
       </c>
       <c r="I50">
@@ -2409,7 +2457,7 @@
       <c r="B51" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="3">
         <v>609</v>
       </c>
       <c r="D51" s="1" t="s">
@@ -2418,6 +2466,9 @@
       <c r="E51" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -2426,13 +2477,13 @@
       <c r="B52" t="s">
         <v>92</v>
       </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52">
-        <v>1</v>
-      </c>
-      <c r="H52">
+      <c r="F52" s="4">
+        <v>1</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1</v>
+      </c>
+      <c r="H52" s="4">
         <v>16</v>
       </c>
       <c r="I52">
@@ -2452,13 +2503,13 @@
       <c r="B53" t="s">
         <v>93</v>
       </c>
-      <c r="F53">
-        <v>3</v>
-      </c>
-      <c r="G53">
-        <v>1</v>
-      </c>
-      <c r="H53">
+      <c r="F53" s="4">
+        <v>3</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1</v>
+      </c>
+      <c r="H53" s="4">
         <v>16</v>
       </c>
       <c r="I53">
@@ -2478,13 +2529,13 @@
       <c r="B54" t="s">
         <v>94</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="4">
         <v>5</v>
       </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54">
+      <c r="G54" s="4">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4">
         <v>16</v>
       </c>
       <c r="I54">
@@ -2504,7 +2555,7 @@
       <c r="B55" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55" s="3">
         <v>610</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -2513,6 +2564,9 @@
       <c r="E55" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -2521,13 +2575,13 @@
       <c r="B56" t="s">
         <v>95</v>
       </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56">
+      <c r="F56" s="4">
+        <v>1</v>
+      </c>
+      <c r="G56" s="4">
+        <v>1</v>
+      </c>
+      <c r="H56" s="4">
         <v>16</v>
       </c>
       <c r="I56">
@@ -2547,13 +2601,13 @@
       <c r="B57" t="s">
         <v>96</v>
       </c>
-      <c r="F57">
-        <v>3</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="H57">
+      <c r="F57" s="4">
+        <v>3</v>
+      </c>
+      <c r="G57" s="4">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4">
         <v>16</v>
       </c>
       <c r="I57">
@@ -2573,13 +2627,13 @@
       <c r="B58" t="s">
         <v>97</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="4">
         <v>5</v>
       </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58">
+      <c r="G58" s="4">
+        <v>1</v>
+      </c>
+      <c r="H58" s="4">
         <v>16</v>
       </c>
       <c r="I58">
@@ -2599,7 +2653,7 @@
       <c r="B59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="3">
         <v>704</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -2608,6 +2662,9 @@
       <c r="E59" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -2616,13 +2673,13 @@
       <c r="B60" t="s">
         <v>98</v>
       </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60">
+      <c r="F60" s="4">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4">
+        <v>1</v>
+      </c>
+      <c r="H60" s="4">
         <v>16</v>
       </c>
       <c r="I60">
@@ -2639,13 +2696,13 @@
       <c r="B61" t="s">
         <v>99</v>
       </c>
-      <c r="F61">
-        <v>3</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61">
+      <c r="F61" s="4">
+        <v>3</v>
+      </c>
+      <c r="G61" s="4">
+        <v>1</v>
+      </c>
+      <c r="H61" s="4">
         <v>16</v>
       </c>
       <c r="I61">
@@ -2662,7 +2719,7 @@
       <c r="B62" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62" s="3">
         <v>705</v>
       </c>
       <c r="D62" s="1" t="s">
@@ -2671,6 +2728,9 @@
       <c r="E62" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -2679,13 +2739,13 @@
       <c r="B63" t="s">
         <v>100</v>
       </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63">
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4">
         <v>16</v>
       </c>
       <c r="I63">
@@ -2702,13 +2762,13 @@
       <c r="B64" t="s">
         <v>101</v>
       </c>
-      <c r="F64">
-        <v>3</v>
-      </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
-      <c r="H64">
+      <c r="F64" s="4">
+        <v>3</v>
+      </c>
+      <c r="G64" s="4">
+        <v>1</v>
+      </c>
+      <c r="H64" s="4">
         <v>16</v>
       </c>
       <c r="I64">
@@ -2725,7 +2785,7 @@
       <c r="B65" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65" s="3">
         <v>706</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -2734,6 +2794,9 @@
       <c r="E65" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -2742,13 +2805,13 @@
       <c r="B66" t="s">
         <v>102</v>
       </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66">
-        <v>1</v>
-      </c>
-      <c r="H66">
+      <c r="F66" s="4">
+        <v>1</v>
+      </c>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+      <c r="H66" s="4">
         <v>16</v>
       </c>
       <c r="I66">
@@ -2765,13 +2828,13 @@
       <c r="B67" t="s">
         <v>103</v>
       </c>
-      <c r="F67">
-        <v>3</v>
-      </c>
-      <c r="G67">
-        <v>1</v>
-      </c>
-      <c r="H67">
+      <c r="F67" s="4">
+        <v>3</v>
+      </c>
+      <c r="G67" s="4">
+        <v>1</v>
+      </c>
+      <c r="H67" s="4">
         <v>16</v>
       </c>
       <c r="I67">
@@ -2788,7 +2851,7 @@
       <c r="B68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C68" s="3">
         <v>448</v>
       </c>
       <c r="D68" s="1" t="s">
@@ -2797,6 +2860,9 @@
       <c r="E68" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -2805,13 +2871,13 @@
       <c r="B69" t="s">
         <v>104</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="4">
         <v>7</v>
       </c>
-      <c r="G69">
-        <v>1</v>
-      </c>
-      <c r="H69">
+      <c r="G69" s="4">
+        <v>1</v>
+      </c>
+      <c r="H69" s="4">
         <v>1</v>
       </c>
       <c r="I69" t="s">
@@ -2825,7 +2891,7 @@
       <c r="B70" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C70" s="3">
         <v>449</v>
       </c>
       <c r="D70" s="1" t="s">
@@ -2834,6 +2900,9 @@
       <c r="E70" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -2842,13 +2911,13 @@
       <c r="B71" t="s">
         <v>108</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="4">
         <v>7</v>
       </c>
-      <c r="G71">
-        <v>1</v>
-      </c>
-      <c r="H71">
+      <c r="G71" s="4">
+        <v>1</v>
+      </c>
+      <c r="H71" s="4">
         <v>1</v>
       </c>
       <c r="I71" t="s">
@@ -2862,7 +2931,7 @@
       <c r="B72" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="3">
         <v>450</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -2871,6 +2940,9 @@
       <c r="E72" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
@@ -2879,13 +2951,13 @@
       <c r="B73" t="s">
         <v>109</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="4">
         <v>7</v>
       </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-      <c r="H73">
+      <c r="G73" s="4">
+        <v>1</v>
+      </c>
+      <c r="H73" s="4">
         <v>1</v>
       </c>
       <c r="I73" t="s">
@@ -2899,7 +2971,7 @@
       <c r="B74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C74" s="1">
+      <c r="C74" s="3">
         <v>192</v>
       </c>
       <c r="D74" s="1" t="s">
@@ -2908,6 +2980,9 @@
       <c r="E74" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -2916,13 +2991,13 @@
       <c r="B75" t="s">
         <v>111</v>
       </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-      <c r="H75">
+      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="G75" s="4">
+        <v>1</v>
+      </c>
+      <c r="H75" s="4">
         <v>1</v>
       </c>
       <c r="I75" t="s">
@@ -2936,13 +3011,13 @@
       <c r="B76" t="s">
         <v>112</v>
       </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
-      <c r="H76">
+      <c r="F76" s="4">
+        <v>1</v>
+      </c>
+      <c r="G76" s="4">
+        <v>2</v>
+      </c>
+      <c r="H76" s="4">
         <v>1</v>
       </c>
       <c r="I76" t="s">
@@ -2956,13 +3031,13 @@
       <c r="B77" t="s">
         <v>113</v>
       </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-      <c r="G77">
-        <v>3</v>
-      </c>
-      <c r="H77">
+      <c r="F77" s="4">
+        <v>1</v>
+      </c>
+      <c r="G77" s="4">
+        <v>3</v>
+      </c>
+      <c r="H77" s="4">
         <v>1</v>
       </c>
       <c r="I77" t="s">
@@ -2976,13 +3051,13 @@
       <c r="B78" t="s">
         <v>114</v>
       </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78">
+      <c r="F78" s="4">
+        <v>1</v>
+      </c>
+      <c r="G78" s="4">
         <v>4</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="4">
         <v>1</v>
       </c>
       <c r="I78" t="s">
@@ -2996,13 +3071,13 @@
       <c r="B79" t="s">
         <v>115</v>
       </c>
-      <c r="F79">
-        <v>3</v>
-      </c>
-      <c r="G79">
+      <c r="F79" s="4">
+        <v>3</v>
+      </c>
+      <c r="G79" s="4">
         <v>4</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="4">
         <v>1</v>
       </c>
       <c r="I79" t="s">
@@ -3016,13 +3091,13 @@
       <c r="B80" t="s">
         <v>116</v>
       </c>
-      <c r="F80">
-        <v>3</v>
-      </c>
-      <c r="G80">
+      <c r="F80" s="4">
+        <v>3</v>
+      </c>
+      <c r="G80" s="4">
         <v>6</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="4">
         <v>1</v>
       </c>
       <c r="I80" t="s">
@@ -3036,13 +3111,13 @@
       <c r="B81" t="s">
         <v>111</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="4">
         <v>6</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="4">
         <v>4</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="4">
         <v>1</v>
       </c>
       <c r="I81" t="s">
@@ -3056,7 +3131,7 @@
       <c r="B82" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="3">
         <v>193</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -3065,6 +3140,9 @@
       <c r="E82" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
@@ -3073,13 +3151,13 @@
       <c r="B83" t="s">
         <v>117</v>
       </c>
-      <c r="F83">
-        <v>1</v>
-      </c>
-      <c r="G83">
-        <v>1</v>
-      </c>
-      <c r="H83">
+      <c r="F83" s="4">
+        <v>1</v>
+      </c>
+      <c r="G83" s="4">
+        <v>1</v>
+      </c>
+      <c r="H83" s="4">
         <v>1</v>
       </c>
       <c r="I83" t="s">
@@ -3093,13 +3171,13 @@
       <c r="B84" t="s">
         <v>118</v>
       </c>
-      <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84">
-        <v>2</v>
-      </c>
-      <c r="H84">
+      <c r="F84" s="4">
+        <v>1</v>
+      </c>
+      <c r="G84" s="4">
+        <v>2</v>
+      </c>
+      <c r="H84" s="4">
         <v>1</v>
       </c>
       <c r="I84" t="s">
@@ -3113,13 +3191,13 @@
       <c r="B85" t="s">
         <v>119</v>
       </c>
-      <c r="F85">
-        <v>1</v>
-      </c>
-      <c r="G85">
-        <v>3</v>
-      </c>
-      <c r="H85">
+      <c r="F85" s="4">
+        <v>1</v>
+      </c>
+      <c r="G85" s="4">
+        <v>3</v>
+      </c>
+      <c r="H85" s="4">
         <v>1</v>
       </c>
       <c r="I85" t="s">
@@ -3133,13 +3211,13 @@
       <c r="B86" t="s">
         <v>120</v>
       </c>
-      <c r="F86">
-        <v>1</v>
-      </c>
-      <c r="G86">
+      <c r="F86" s="4">
+        <v>1</v>
+      </c>
+      <c r="G86" s="4">
         <v>4</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="4">
         <v>1</v>
       </c>
       <c r="I86" t="s">
@@ -3153,13 +3231,13 @@
       <c r="B87" t="s">
         <v>121</v>
       </c>
-      <c r="F87">
-        <v>3</v>
-      </c>
-      <c r="G87">
+      <c r="F87" s="4">
+        <v>3</v>
+      </c>
+      <c r="G87" s="4">
         <v>4</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="4">
         <v>1</v>
       </c>
       <c r="I87" t="s">
@@ -3173,13 +3251,13 @@
       <c r="B88" t="s">
         <v>122</v>
       </c>
-      <c r="F88">
-        <v>3</v>
-      </c>
-      <c r="G88">
+      <c r="F88" s="4">
+        <v>3</v>
+      </c>
+      <c r="G88" s="4">
         <v>6</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="4">
         <v>1</v>
       </c>
       <c r="I88" t="s">
@@ -3193,13 +3271,13 @@
       <c r="B89" t="s">
         <v>117</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="4">
         <v>6</v>
       </c>
-      <c r="G89">
+      <c r="G89" s="4">
         <v>4</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="4">
         <v>1</v>
       </c>
       <c r="I89" t="s">
@@ -3213,7 +3291,7 @@
       <c r="B90" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C90" s="1">
+      <c r="C90" s="3">
         <v>194</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -3222,6 +3300,9 @@
       <c r="E90" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
@@ -3230,13 +3311,13 @@
       <c r="B91" t="s">
         <v>123</v>
       </c>
-      <c r="F91">
-        <v>1</v>
-      </c>
-      <c r="G91">
-        <v>1</v>
-      </c>
-      <c r="H91">
+      <c r="F91" s="4">
+        <v>1</v>
+      </c>
+      <c r="G91" s="4">
+        <v>1</v>
+      </c>
+      <c r="H91" s="4">
         <v>1</v>
       </c>
       <c r="I91" t="s">
@@ -3250,13 +3331,13 @@
       <c r="B92" t="s">
         <v>124</v>
       </c>
-      <c r="F92">
-        <v>1</v>
-      </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
-      <c r="H92">
+      <c r="F92" s="4">
+        <v>1</v>
+      </c>
+      <c r="G92" s="4">
+        <v>2</v>
+      </c>
+      <c r="H92" s="4">
         <v>1</v>
       </c>
       <c r="I92" t="s">
@@ -3270,13 +3351,13 @@
       <c r="B93" t="s">
         <v>125</v>
       </c>
-      <c r="F93">
-        <v>1</v>
-      </c>
-      <c r="G93">
-        <v>3</v>
-      </c>
-      <c r="H93">
+      <c r="F93" s="4">
+        <v>1</v>
+      </c>
+      <c r="G93" s="4">
+        <v>3</v>
+      </c>
+      <c r="H93" s="4">
         <v>1</v>
       </c>
       <c r="I93" t="s">
@@ -3290,13 +3371,13 @@
       <c r="B94" t="s">
         <v>126</v>
       </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94">
+      <c r="F94" s="4">
+        <v>1</v>
+      </c>
+      <c r="G94" s="4">
         <v>4</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="4">
         <v>1</v>
       </c>
       <c r="I94" t="s">
@@ -3310,13 +3391,13 @@
       <c r="B95" t="s">
         <v>127</v>
       </c>
-      <c r="F95">
-        <v>3</v>
-      </c>
-      <c r="G95">
+      <c r="F95" s="4">
+        <v>3</v>
+      </c>
+      <c r="G95" s="4">
         <v>4</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="4">
         <v>1</v>
       </c>
       <c r="I95" t="s">
@@ -3330,13 +3411,13 @@
       <c r="B96" t="s">
         <v>128</v>
       </c>
-      <c r="F96">
-        <v>3</v>
-      </c>
-      <c r="G96">
+      <c r="F96" s="4">
+        <v>3</v>
+      </c>
+      <c r="G96" s="4">
         <v>6</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="4">
         <v>1</v>
       </c>
       <c r="I96" t="s">
@@ -3350,13 +3431,13 @@
       <c r="B97" t="s">
         <v>123</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="4">
         <v>6</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="4">
         <v>4</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="4">
         <v>1</v>
       </c>
       <c r="I97" t="s">
@@ -3370,7 +3451,7 @@
       <c r="B98" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C98" s="1">
+      <c r="C98" s="3">
         <v>224</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -3379,6 +3460,9 @@
       <c r="E98" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
     </row>
     <row r="99" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
@@ -3387,7 +3471,7 @@
       <c r="B99" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C99" s="3">
         <v>225</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -3396,6 +3480,9 @@
       <c r="E99" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
     </row>
     <row r="100" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
@@ -3404,7 +3491,7 @@
       <c r="B100" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C100" s="1">
+      <c r="C100" s="3">
         <v>226</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -3413,6 +3500,9 @@
       <c r="E100" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
     </row>
     <row r="101" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
@@ -3421,7 +3511,7 @@
       <c r="B101" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C101" s="3">
         <v>544</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -3430,6 +3520,9 @@
       <c r="E101" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
@@ -3438,13 +3531,13 @@
       <c r="B102" t="s">
         <v>76</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="4">
         <v>5</v>
       </c>
-      <c r="G102">
-        <v>1</v>
-      </c>
-      <c r="H102">
+      <c r="G102" s="4">
+        <v>1</v>
+      </c>
+      <c r="H102" s="4">
         <v>16</v>
       </c>
       <c r="I102">
@@ -3464,7 +3557,7 @@
       <c r="B103" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C103" s="3">
         <v>545</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -3473,6 +3566,9 @@
       <c r="E103" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
@@ -3481,13 +3577,13 @@
       <c r="B104" t="s">
         <v>77</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="4">
         <v>5</v>
       </c>
-      <c r="G104">
-        <v>1</v>
-      </c>
-      <c r="H104">
+      <c r="G104" s="4">
+        <v>1</v>
+      </c>
+      <c r="H104" s="4">
         <v>16</v>
       </c>
       <c r="I104">
@@ -3507,7 +3603,7 @@
       <c r="B105" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C105" s="1">
+      <c r="C105" s="3">
         <v>546</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -3516,6 +3612,9 @@
       <c r="E105" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
@@ -3524,13 +3623,13 @@
       <c r="B106" t="s">
         <v>78</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="4">
         <v>5</v>
       </c>
-      <c r="G106">
-        <v>1</v>
-      </c>
-      <c r="H106">
+      <c r="G106" s="4">
+        <v>1</v>
+      </c>
+      <c r="H106" s="4">
         <v>16</v>
       </c>
       <c r="I106">
@@ -3550,7 +3649,7 @@
       <c r="B107" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C107" s="1">
+      <c r="C107" s="3">
         <v>576</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -3559,6 +3658,9 @@
       <c r="E107" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
@@ -3567,13 +3669,13 @@
       <c r="B108" t="s">
         <v>66</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="4">
         <v>5</v>
       </c>
-      <c r="G108">
-        <v>1</v>
-      </c>
-      <c r="H108">
+      <c r="G108" s="4">
+        <v>1</v>
+      </c>
+      <c r="H108" s="4">
         <v>16</v>
       </c>
       <c r="I108">
@@ -3593,7 +3695,7 @@
       <c r="B109" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C109" s="1">
+      <c r="C109" s="3">
         <v>577</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -3602,6 +3704,9 @@
       <c r="E109" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+      <c r="H109" s="3"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
@@ -3610,13 +3715,13 @@
       <c r="B110" t="s">
         <v>67</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="4">
         <v>5</v>
       </c>
-      <c r="G110">
-        <v>1</v>
-      </c>
-      <c r="H110">
+      <c r="G110" s="4">
+        <v>1</v>
+      </c>
+      <c r="H110" s="4">
         <v>16</v>
       </c>
       <c r="I110">
@@ -3636,7 +3741,7 @@
       <c r="B111" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111" s="3">
         <v>578</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -3645,6 +3750,9 @@
       <c r="E111" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
@@ -3653,13 +3761,13 @@
       <c r="B112" t="s">
         <v>68</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="4">
         <v>5</v>
       </c>
-      <c r="G112">
-        <v>1</v>
-      </c>
-      <c r="H112">
+      <c r="G112" s="4">
+        <v>1</v>
+      </c>
+      <c r="H112" s="4">
         <v>16</v>
       </c>
       <c r="I112">

</xml_diff>

<commit_message>
Am now able to put it all together and have all the needed files generating. Just need to format the output a little more then we'll move on.
</commit_message>
<xml_diff>
--- a/StdCANSheet_Updated.xlsx
+++ b/StdCANSheet_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\quickScripts\PythonPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252778D2-1517-4BF1-8DDA-2E3A4E3E6E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9790787-C50A-41FB-ADBD-9546C49DAA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StdCANSheet_Updated" sheetId="1" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,7 +1423,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>59</v>
@@ -1521,7 +1521,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>59</v>

</xml_diff>